<commit_message>
Updated Documents with most recent version
</commit_message>
<xml_diff>
--- a/Our Team/Bios (Responses).xlsx
+++ b/Our Team/Bios (Responses).xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="61">
   <si>
     <t>Timestamp</t>
   </si>
@@ -188,6 +188,25 @@
   </si>
   <si>
     <t>Ones that don't call back even when they said they would and you know you both had a really great time that one night.</t>
+  </si>
+  <si>
+    <t>I'm Steven Sewell, I found this project stagnant and am now assigning myself to position of community manager in hopes of putting some fuel into this machine.</t>
+  </si>
+  <si>
+    <t>I am a labor worker for conventions to pay the bills, an entrepreneur by past experience, and I've been playing a lot of Minecraft lately.</t>
+  </si>
+  <si>
+    <t>Because doing what other people want to you to do sucks.</t>
+  </si>
+  <si>
+    <t>Chase conspiracy theories down strange rabbit holes and did I mention Minecraft?</t>
+  </si>
+  <si>
+    <t>Email: Stevenhasspam@gmail.com
+Cell #: 714-552-9943</t>
+  </si>
+  <si>
+    <t>A tomato (because it's a fruit!)</t>
   </si>
   <si>
     <t>Cortney Robinson</t>
@@ -258,7 +277,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment wrapText="1"/>
     </xf>
@@ -269,6 +288,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -508,26 +533,49 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="2">
+      <c r="A10" s="4">
+        <v>42791.772455694445</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2">
         <v>41389.17332175926</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>54</v>
+      <c r="B11" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>